<commit_message>
created diet api endpoints
</commit_message>
<xml_diff>
--- a/Backend/API.xlsx
+++ b/Backend/API.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\287927\Documents\Project\Balance Point\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CBE1A1-B69C-4445-8757-C07A1E1F1F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3393C7D-762B-4A8C-A527-12DEF82CC8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>API Name</t>
   </si>
@@ -118,6 +118,84 @@
   </si>
   <si>
     <t>Retrieve details of a single workout session.</t>
+  </si>
+  <si>
+    <t>/meals/</t>
+  </si>
+  <si>
+    <t>Create a new meal</t>
+  </si>
+  <si>
+    <t>Retrieve all meals for a user</t>
+  </si>
+  <si>
+    <t>/meals/&lt;meal_id&gt;/</t>
+  </si>
+  <si>
+    <t>Retrieve a specific meal</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>Update an existing meal</t>
+  </si>
+  <si>
+    <t>Delete a meal</t>
+  </si>
+  <si>
+    <t>/food-items/</t>
+  </si>
+  <si>
+    <t>Retrieve all food items</t>
+  </si>
+  <si>
+    <t>Create a new food item</t>
+  </si>
+  <si>
+    <t>/food-items/&lt;id&gt;/</t>
+  </si>
+  <si>
+    <t>Retrieve a specific food item</t>
+  </si>
+  <si>
+    <t>Update an existing food item</t>
+  </si>
+  <si>
+    <t>Delete a food item</t>
+  </si>
+  <si>
+    <t>Create Meal</t>
+  </si>
+  <si>
+    <t>Retrieve All Meals</t>
+  </si>
+  <si>
+    <t>Retrieve Specific Meal</t>
+  </si>
+  <si>
+    <t>Update Meal</t>
+  </si>
+  <si>
+    <t>Delete Meal</t>
+  </si>
+  <si>
+    <t>Retrieve All Food Items</t>
+  </si>
+  <si>
+    <t>Create Food Item</t>
+  </si>
+  <si>
+    <t>Retrieve Specific Food Item</t>
+  </si>
+  <si>
+    <t>Update Food Item</t>
+  </si>
+  <si>
+    <t>Delete Food Item</t>
+  </si>
+  <si>
+    <t>/meals/user/&lt;user_id&gt;</t>
   </si>
 </sst>
 </file>
@@ -464,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -478,7 +556,7 @@
     <col min="4" max="4" width="48.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,6 +694,146 @@
       </c>
       <c r="D10" s="2" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="4" customFormat="1">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="4" customFormat="1">
+      <c r="A15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="4" customFormat="1">
+      <c r="A16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="4" customFormat="1">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="4" customFormat="1">
+      <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="4" customFormat="1">
+      <c r="A19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="4" customFormat="1">
+      <c r="A20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="4" customFormat="1">
+      <c r="A21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="4" customFormat="1">
+      <c r="A22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="4" customFormat="1">
+      <c r="A23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create user model and api endpoints except login and logout
</commit_message>
<xml_diff>
--- a/Backend/API.xlsx
+++ b/Backend/API.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\287927\Documents\Project\Balance Point\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3393C7D-762B-4A8C-A527-12DEF82CC8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2DF26E-E784-4902-A8AE-A6C447ADD180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t>API Name</t>
   </si>
@@ -196,6 +196,60 @@
   </si>
   <si>
     <t>/meals/user/&lt;user_id&gt;</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>/user/register/</t>
+  </si>
+  <si>
+    <t>Creates a new user and a corresponding UserAssessment instance in one request.</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t>/user/login/</t>
+  </si>
+  <si>
+    <t>Authenticates a user and returns a JWT token upon successful login.</t>
+  </si>
+  <si>
+    <t>Sign Out</t>
+  </si>
+  <si>
+    <t>/user/logout/</t>
+  </si>
+  <si>
+    <t>Handles user logout, discarding the JWT token on the client side or blacklisting it if needed.</t>
+  </si>
+  <si>
+    <t>Initiates the password reset process for a user.</t>
+  </si>
+  <si>
+    <t>Password Reset</t>
+  </si>
+  <si>
+    <t>User Profile</t>
+  </si>
+  <si>
+    <t>/user/profile/&lt;id&gt;</t>
+  </si>
+  <si>
+    <t>Retrieves user profile information and UserAssessment instance together in one request.</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>User Assessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updates UserAssessment instance </t>
+  </si>
+  <si>
+    <t>/user/change-password/</t>
   </si>
 </sst>
 </file>
@@ -224,7 +278,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +288,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -262,6 +322,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -836,6 +909,90 @@
         <v>45</v>
       </c>
     </row>
+    <row r="27" spans="1:4" s="4" customFormat="1" ht="29">
+      <c r="A27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="29">
+      <c r="A28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="29">
+      <c r="A29" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="9" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="4" customFormat="1" ht="43.5" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="4" customFormat="1">
+      <c r="A32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added endpoint to get user
</commit_message>
<xml_diff>
--- a/Backend/API.xlsx
+++ b/Backend/API.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\287927\Documents\Project\Balance Point\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD810EF8-D1E2-4F81-B4C8-ACF94C6241E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D539F2F7-1B39-4591-8DE5-113DC0D7B399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="180">
   <si>
     <t>API Name</t>
   </si>
@@ -564,6 +564,18 @@
   </si>
   <si>
     <t>Delete User Assessment</t>
+  </si>
+  <si>
+    <t>npm install @fortawesome/fontawesome-free</t>
+  </si>
+  <si>
+    <t>npm install @nivo/line</t>
+  </si>
+  <si>
+    <t>antd</t>
+  </si>
+  <si>
+    <t>npm install @reduxjs/toolkit react-redux</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1974,6 +1986,26 @@
         <v>165</v>
       </c>
     </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>